<commit_message>
Significant rewrite of conservation of angular momentum lab
Now uses Capstone and a photogate instead of taking a movie and using Tracker--much faster and easier.  Also introduce using masking tape to keep weight from sliding off disk, and rewrote the parts for error analysis.
</commit_message>
<xml_diff>
--- a/StudentGuideModule1/what_labs_to_include/131 lab list for 2021fall.xlsx
+++ b/StudentGuideModule1/what_labs_to_include/131 lab list for 2021fall.xlsx
@@ -1,16 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="21405"/>
-  <workbookPr autoCompressPictures="0"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="20380"/>
+  <workbookPr autoCompressPictures="0" defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mtrawick\Desktop\github\131\StudentGuideModule1\what_labs_to_include\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{859E717C-E9E6-4644-9E39-F4A54A669F82}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16060" tabRatio="539"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25596" windowHeight="16056" tabRatio="539" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="lablist" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet1" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="140001" concurrentCalc="0"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -20,12 +26,12 @@
 </file>
 
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>Matt Trawick</author>
   </authors>
   <commentList>
-    <comment ref="X1" authorId="0">
+    <comment ref="X1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000001000000}">
       <text>
         <r>
           <rPr>
@@ -118,7 +124,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="Y11" authorId="0">
+    <comment ref="Y11" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000002000000}">
       <text>
         <r>
           <rPr>
@@ -171,7 +177,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="Z19" authorId="0">
+    <comment ref="Z19" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000003000000}">
       <text>
         <r>
           <rPr>
@@ -196,7 +202,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="X22" authorId="0">
+    <comment ref="X22" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000004000000}">
       <text>
         <r>
           <rPr>
@@ -229,7 +235,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="Y22" authorId="0">
+    <comment ref="Y22" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000005000000}">
       <text>
         <r>
           <rPr>
@@ -253,7 +259,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AA22" authorId="0">
+    <comment ref="AA22" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000006000000}">
       <text>
         <r>
           <rPr>
@@ -278,7 +284,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="N61" authorId="0">
+    <comment ref="N61" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000007000000}">
       <text>
         <r>
           <rPr>
@@ -307,7 +313,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="217" uniqueCount="211">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="218" uniqueCount="212">
   <si>
     <t>1 Music to Our Ears: Standing Waves in Strings 7</t>
   </si>
@@ -942,14 +948,17 @@
   </si>
   <si>
     <t>2017 fall Alina</t>
+  </si>
+  <si>
+    <t>Updated by Matt in 2021</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
   <fonts count="24" x14ac:knownFonts="1">
     <font>
@@ -1599,7 +1608,7 @@
     <xf numFmtId="0" fontId="1" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -1616,11 +1625,11 @@
     </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="164" fontId="16" fillId="0" borderId="12" xfId="42" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="44" fontId="16" fillId="0" borderId="12" xfId="42" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="14" xfId="42" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="16" xfId="42" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="14" xfId="42" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="16" xfId="42" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
@@ -1634,7 +1643,7 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="12" xfId="42" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="12" xfId="42" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1"/>
@@ -2211,33 +2220,33 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AE123"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B25" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="85" workbookViewId="0">
-      <selection activeCell="T65" sqref="T65"/>
+    <sheetView tabSelected="1" topLeftCell="B13" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="85" workbookViewId="0">
+      <selection activeCell="I60" sqref="I60"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="18.83203125" style="10" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="18.77734375" style="10" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="46.33203125" style="22" customWidth="1"/>
-    <col min="3" max="3" width="8.1640625" style="13" customWidth="1"/>
-    <col min="4" max="8" width="5.83203125" style="13" customWidth="1"/>
-    <col min="9" max="9" width="28.5" style="19" customWidth="1"/>
-    <col min="10" max="11" width="10.1640625" style="34" customWidth="1"/>
-    <col min="12" max="18" width="8.83203125" style="34" customWidth="1"/>
-    <col min="19" max="19" width="9.1640625" style="34" customWidth="1"/>
-    <col min="20" max="20" width="8.83203125" style="34" customWidth="1"/>
-    <col min="21" max="21" width="8.83203125" style="2" customWidth="1"/>
+    <col min="3" max="3" width="8.109375" style="13" customWidth="1"/>
+    <col min="4" max="8" width="5.77734375" style="13" customWidth="1"/>
+    <col min="9" max="9" width="28.44140625" style="19" customWidth="1"/>
+    <col min="10" max="11" width="10.109375" style="34" customWidth="1"/>
+    <col min="12" max="18" width="8.77734375" style="34" customWidth="1"/>
+    <col min="19" max="19" width="9.109375" style="34" customWidth="1"/>
+    <col min="20" max="20" width="8.77734375" style="34" customWidth="1"/>
+    <col min="21" max="21" width="8.77734375" style="2" customWidth="1"/>
     <col min="22" max="22" width="11" style="3" customWidth="1"/>
-    <col min="23" max="23" width="2.5" style="3" customWidth="1"/>
+    <col min="23" max="23" width="2.44140625" style="3" customWidth="1"/>
     <col min="24" max="24" width="10.33203125" style="3" customWidth="1"/>
-    <col min="26" max="26" width="9.5" customWidth="1"/>
-    <col min="27" max="27" width="10.1640625" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="9.44140625" customWidth="1"/>
+    <col min="27" max="27" width="10.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:31" s="1" customFormat="1" ht="28">
+    <row r="1" spans="1:31" s="1" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A1" s="46" t="s">
         <v>73</v>
       </c>
@@ -2314,7 +2323,7 @@
       <c r="AD1" s="31"/>
       <c r="AE1" s="31"/>
     </row>
-    <row r="2" spans="1:31" s="1" customFormat="1">
+    <row r="2" spans="1:31" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A2" s="10" t="s">
         <v>86</v>
       </c>
@@ -2360,7 +2369,7 @@
       <c r="AD2" s="31"/>
       <c r="AE2" s="31"/>
     </row>
-    <row r="3" spans="1:31" s="1" customFormat="1">
+    <row r="3" spans="1:31" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A3" s="46"/>
       <c r="B3" s="52" t="s">
         <v>88</v>
@@ -2404,7 +2413,7 @@
       <c r="AD3" s="31"/>
       <c r="AE3" s="31"/>
     </row>
-    <row r="4" spans="1:31" s="1" customFormat="1">
+    <row r="4" spans="1:31" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A4" s="28" t="s">
         <v>110</v>
       </c>
@@ -2464,7 +2473,7 @@
       <c r="AD4" s="31"/>
       <c r="AE4" s="31"/>
     </row>
-    <row r="5" spans="1:31">
+    <row r="5" spans="1:31" x14ac:dyDescent="0.3">
       <c r="B5" s="22" t="s">
         <v>120</v>
       </c>
@@ -2493,7 +2502,7 @@
       <c r="AD5" s="31"/>
       <c r="AE5" s="31"/>
     </row>
-    <row r="6" spans="1:31">
+    <row r="6" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A6" s="28"/>
       <c r="B6" s="29" t="s">
         <v>121</v>
@@ -2520,7 +2529,7 @@
       <c r="AD6" s="31"/>
       <c r="AE6" s="31"/>
     </row>
-    <row r="7" spans="1:31" s="31" customFormat="1">
+    <row r="7" spans="1:31" s="31" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A7" s="10"/>
       <c r="B7" s="22" t="s">
         <v>122</v>
@@ -2558,7 +2567,7 @@
       <c r="Z7" s="5"/>
       <c r="AA7" s="14"/>
     </row>
-    <row r="8" spans="1:31">
+    <row r="8" spans="1:31" x14ac:dyDescent="0.3">
       <c r="B8" s="22" t="s">
         <v>123</v>
       </c>
@@ -2584,7 +2593,7 @@
       <c r="AD8" s="31"/>
       <c r="AE8" s="31"/>
     </row>
-    <row r="9" spans="1:31">
+    <row r="9" spans="1:31" x14ac:dyDescent="0.3">
       <c r="B9" s="22" t="s">
         <v>124</v>
       </c>
@@ -2649,7 +2658,7 @@
       <c r="AD9" s="31"/>
       <c r="AE9" s="31"/>
     </row>
-    <row r="10" spans="1:31" ht="15" thickBot="1">
+    <row r="10" spans="1:31" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B10" s="22" t="s">
         <v>125</v>
       </c>
@@ -2714,7 +2723,7 @@
       <c r="AD10" s="31"/>
       <c r="AE10" s="31"/>
     </row>
-    <row r="11" spans="1:31">
+    <row r="11" spans="1:31" x14ac:dyDescent="0.3">
       <c r="B11" s="22" t="s">
         <v>126</v>
       </c>
@@ -2778,7 +2787,7 @@
       <c r="AD11" s="31"/>
       <c r="AE11" s="31"/>
     </row>
-    <row r="12" spans="1:31" ht="15" thickBot="1">
+    <row r="12" spans="1:31" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B12" s="22" t="s">
         <v>127</v>
       </c>
@@ -2806,7 +2815,7 @@
       <c r="AD12" s="31"/>
       <c r="AE12" s="31"/>
     </row>
-    <row r="13" spans="1:31">
+    <row r="13" spans="1:31" x14ac:dyDescent="0.3">
       <c r="B13" s="22" t="s">
         <v>175</v>
       </c>
@@ -2865,7 +2874,7 @@
       <c r="AD13" s="31"/>
       <c r="AE13" s="31"/>
     </row>
-    <row r="14" spans="1:31" ht="15" thickBot="1">
+    <row r="14" spans="1:31" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B14" s="22" t="s">
         <v>128</v>
       </c>
@@ -2925,7 +2934,7 @@
       <c r="AD14" s="31"/>
       <c r="AE14" s="31"/>
     </row>
-    <row r="15" spans="1:31">
+    <row r="15" spans="1:31" x14ac:dyDescent="0.3">
       <c r="B15" s="22" t="s">
         <v>174</v>
       </c>
@@ -2958,7 +2967,7 @@
       <c r="AD15" s="31"/>
       <c r="AE15" s="31"/>
     </row>
-    <row r="16" spans="1:31">
+    <row r="16" spans="1:31" x14ac:dyDescent="0.3">
       <c r="B16" s="22" t="s">
         <v>129</v>
       </c>
@@ -2991,7 +3000,7 @@
       <c r="AD16" s="31"/>
       <c r="AE16" s="31"/>
     </row>
-    <row r="17" spans="1:31">
+    <row r="17" spans="1:31" x14ac:dyDescent="0.3">
       <c r="B17" s="22" t="s">
         <v>130</v>
       </c>
@@ -3042,7 +3051,7 @@
       <c r="AD17" s="31"/>
       <c r="AE17" s="31"/>
     </row>
-    <row r="18" spans="1:31">
+    <row r="18" spans="1:31" x14ac:dyDescent="0.3">
       <c r="B18" s="22" t="s">
         <v>131</v>
       </c>
@@ -3105,7 +3114,7 @@
       <c r="AD18" s="31"/>
       <c r="AE18" s="31"/>
     </row>
-    <row r="19" spans="1:31" ht="15" thickBot="1">
+    <row r="19" spans="1:31" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B19" s="22" t="s">
         <v>132</v>
       </c>
@@ -3138,7 +3147,7 @@
       <c r="AD19" s="31"/>
       <c r="AE19" s="31"/>
     </row>
-    <row r="20" spans="1:31">
+    <row r="20" spans="1:31" x14ac:dyDescent="0.3">
       <c r="B20" s="22" t="s">
         <v>133</v>
       </c>
@@ -3161,7 +3170,7 @@
       <c r="AD20" s="31"/>
       <c r="AE20" s="31"/>
     </row>
-    <row r="21" spans="1:31" ht="15" thickBot="1">
+    <row r="21" spans="1:31" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B21" s="22" t="s">
         <v>134</v>
       </c>
@@ -3187,7 +3196,7 @@
       <c r="AD21" s="31"/>
       <c r="AE21" s="31"/>
     </row>
-    <row r="22" spans="1:31">
+    <row r="22" spans="1:31" x14ac:dyDescent="0.3">
       <c r="B22" s="22" t="s">
         <v>135</v>
       </c>
@@ -3221,7 +3230,7 @@
       <c r="AD22" s="31"/>
       <c r="AE22" s="31"/>
     </row>
-    <row r="23" spans="1:31">
+    <row r="23" spans="1:31" x14ac:dyDescent="0.3">
       <c r="B23" s="22" t="s">
         <v>136</v>
       </c>
@@ -3243,7 +3252,7 @@
       </c>
       <c r="Y23" s="6">
         <f t="shared" ref="Y23:Y31" si="1">SUMIF(V$2:V$82,"&gt;=" &amp; X23,C$2:C$82)</f>
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="Z23" s="6">
         <f t="shared" ref="Z23:Z31" si="2">SUMIF(V$2:V$82,"&gt;=" &amp; X23,D$2:D$82)</f>
@@ -3251,14 +3260,14 @@
       </c>
       <c r="AA23" s="8">
         <f t="shared" ref="AA23:AA31" si="3">($Z$17 + $Z$15*Y23+$Z$16*Z23)*(1+Z$18+Z$19)</f>
-        <v>29.64</v>
+        <v>29.574999999999999</v>
       </c>
       <c r="AB23" s="31"/>
       <c r="AC23" s="31"/>
       <c r="AD23" s="31"/>
       <c r="AE23" s="31"/>
     </row>
-    <row r="24" spans="1:31" s="6" customFormat="1">
+    <row r="24" spans="1:31" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A24" s="10"/>
       <c r="B24" s="22" t="s">
         <v>137</v>
@@ -3322,7 +3331,7 @@
       </c>
       <c r="Y24" s="6">
         <f t="shared" si="1"/>
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="Z24" s="6">
         <f t="shared" si="2"/>
@@ -3330,14 +3339,14 @@
       </c>
       <c r="AA24" s="8">
         <f t="shared" si="3"/>
-        <v>21.45</v>
+        <v>21.385000000000005</v>
       </c>
       <c r="AB24" s="31"/>
       <c r="AC24" s="31"/>
       <c r="AD24" s="31"/>
       <c r="AE24" s="31"/>
     </row>
-    <row r="25" spans="1:31">
+    <row r="25" spans="1:31" x14ac:dyDescent="0.3">
       <c r="B25" s="22" t="s">
         <v>138</v>
       </c>
@@ -3381,7 +3390,7 @@
       </c>
       <c r="Y25" s="6">
         <f t="shared" si="1"/>
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="Z25" s="6">
         <f t="shared" si="2"/>
@@ -3389,14 +3398,14 @@
       </c>
       <c r="AA25" s="8">
         <f t="shared" si="3"/>
-        <v>19.305</v>
+        <v>19.240000000000002</v>
       </c>
       <c r="AB25" s="31"/>
       <c r="AC25" s="31"/>
       <c r="AD25" s="31"/>
       <c r="AE25" s="31"/>
     </row>
-    <row r="26" spans="1:31">
+    <row r="26" spans="1:31" x14ac:dyDescent="0.3">
       <c r="B26" s="22" t="s">
         <v>139</v>
       </c>
@@ -3448,7 +3457,7 @@
       </c>
       <c r="Y26" s="29">
         <f t="shared" si="1"/>
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="Z26" s="29">
         <f t="shared" si="2"/>
@@ -3456,14 +3465,14 @@
       </c>
       <c r="AA26" s="8">
         <f t="shared" si="3"/>
-        <v>18.07</v>
+        <v>18.004999999999999</v>
       </c>
       <c r="AB26" s="31"/>
       <c r="AC26" s="31"/>
       <c r="AD26" s="31"/>
       <c r="AE26" s="31"/>
     </row>
-    <row r="27" spans="1:31">
+    <row r="27" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A27" s="11" t="s">
         <v>117</v>
       </c>
@@ -3527,7 +3536,7 @@
       </c>
       <c r="Y27" s="6">
         <f t="shared" si="1"/>
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="Z27" s="6">
         <f t="shared" si="2"/>
@@ -3535,10 +3544,10 @@
       </c>
       <c r="AA27" s="8">
         <f t="shared" si="3"/>
-        <v>15.535</v>
-      </c>
-    </row>
-    <row r="28" spans="1:31">
+        <v>15.47</v>
+      </c>
+    </row>
+    <row r="28" spans="1:31" x14ac:dyDescent="0.3">
       <c r="B28" s="22" t="s">
         <v>141</v>
       </c>
@@ -3590,7 +3599,7 @@
       </c>
       <c r="Y28" s="6">
         <f t="shared" si="1"/>
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="Z28" s="6">
         <f t="shared" si="2"/>
@@ -3598,10 +3607,10 @@
       </c>
       <c r="AA28" s="8">
         <f t="shared" si="3"/>
-        <v>7.2800000000000011</v>
-      </c>
-    </row>
-    <row r="29" spans="1:31">
+        <v>7.2149999999999999</v>
+      </c>
+    </row>
+    <row r="29" spans="1:31" x14ac:dyDescent="0.3">
       <c r="B29" s="22" t="s">
         <v>142</v>
       </c>
@@ -3632,7 +3641,7 @@
       </c>
       <c r="Y29" s="6">
         <f t="shared" si="1"/>
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="Z29" s="6">
         <f t="shared" si="2"/>
@@ -3640,10 +3649,10 @@
       </c>
       <c r="AA29" s="8">
         <f t="shared" si="3"/>
-        <v>7.02</v>
-      </c>
-    </row>
-    <row r="30" spans="1:31">
+        <v>6.955000000000001</v>
+      </c>
+    </row>
+    <row r="30" spans="1:31" x14ac:dyDescent="0.3">
       <c r="B30" s="22" t="s">
         <v>143</v>
       </c>
@@ -3706,7 +3715,7 @@
         <v>4.2250000000000005</v>
       </c>
     </row>
-    <row r="31" spans="1:31" ht="15" thickBot="1">
+    <row r="31" spans="1:31" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B31" s="22" t="s">
         <v>191</v>
       </c>
@@ -3747,7 +3756,7 @@
         <v>4.2250000000000005</v>
       </c>
     </row>
-    <row r="32" spans="1:31" s="6" customFormat="1">
+    <row r="32" spans="1:31" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A32" s="10"/>
       <c r="B32" s="22" t="s">
         <v>144</v>
@@ -3806,7 +3815,7 @@
       <c r="Y32"/>
       <c r="Z32"/>
     </row>
-    <row r="33" spans="1:31">
+    <row r="33" spans="1:31" x14ac:dyDescent="0.3">
       <c r="B33" s="22" t="s">
         <v>145</v>
       </c>
@@ -3836,7 +3845,7 @@
       </c>
       <c r="W33" s="14"/>
     </row>
-    <row r="34" spans="1:31">
+    <row r="34" spans="1:31" x14ac:dyDescent="0.3">
       <c r="B34" s="22" t="s">
         <v>146</v>
       </c>
@@ -3887,7 +3896,7 @@
       </c>
       <c r="W34" s="14"/>
     </row>
-    <row r="35" spans="1:31">
+    <row r="35" spans="1:31" x14ac:dyDescent="0.3">
       <c r="B35" s="22" t="s">
         <v>147</v>
       </c>
@@ -3922,7 +3931,7 @@
       <c r="W35" s="14"/>
       <c r="X35" s="77"/>
     </row>
-    <row r="36" spans="1:31" s="31" customFormat="1">
+    <row r="36" spans="1:31" s="31" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A36" s="10"/>
       <c r="B36" s="22" t="s">
         <v>194</v>
@@ -3961,7 +3970,7 @@
       <c r="W36" s="14"/>
       <c r="X36" s="77"/>
     </row>
-    <row r="37" spans="1:31">
+    <row r="37" spans="1:31" x14ac:dyDescent="0.3">
       <c r="B37" s="22" t="s">
         <v>148</v>
       </c>
@@ -4010,7 +4019,7 @@
       <c r="W37" s="14"/>
       <c r="X37" s="77"/>
     </row>
-    <row r="38" spans="1:31" s="31" customFormat="1">
+    <row r="38" spans="1:31" s="31" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A38" s="10"/>
       <c r="B38" s="22" t="s">
         <v>149</v>
@@ -4065,7 +4074,7 @@
       <c r="W38" s="14"/>
       <c r="X38" s="77"/>
     </row>
-    <row r="39" spans="1:31">
+    <row r="39" spans="1:31" x14ac:dyDescent="0.3">
       <c r="B39" s="22" t="s">
         <v>150</v>
       </c>
@@ -4103,7 +4112,7 @@
       <c r="X39" s="77"/>
       <c r="AA39" s="6"/>
     </row>
-    <row r="40" spans="1:31">
+    <row r="40" spans="1:31" x14ac:dyDescent="0.3">
       <c r="B40" s="22" t="s">
         <v>180</v>
       </c>
@@ -4126,7 +4135,7 @@
       </c>
       <c r="W40" s="14"/>
     </row>
-    <row r="41" spans="1:31">
+    <row r="41" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A41" s="11" t="s">
         <v>116</v>
       </c>
@@ -4188,7 +4197,7 @@
       <c r="X41" s="14"/>
       <c r="Y41" s="6"/>
     </row>
-    <row r="42" spans="1:31" s="6" customFormat="1">
+    <row r="42" spans="1:31" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A42" s="28"/>
       <c r="B42" s="29" t="s">
         <v>152</v>
@@ -4255,7 +4264,7 @@
       <c r="AD42"/>
       <c r="AE42"/>
     </row>
-    <row r="43" spans="1:31">
+    <row r="43" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A43" s="28"/>
       <c r="B43" s="29" t="s">
         <v>153</v>
@@ -4314,7 +4323,7 @@
       <c r="AD43" s="6"/>
       <c r="AE43" s="6"/>
     </row>
-    <row r="44" spans="1:31">
+    <row r="44" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A44" s="28"/>
       <c r="B44" s="29" t="s">
         <v>154</v>
@@ -4343,7 +4352,7 @@
       <c r="W44" s="14"/>
       <c r="AA44" s="6"/>
     </row>
-    <row r="45" spans="1:31">
+    <row r="45" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A45" s="28"/>
       <c r="B45" s="29" t="s">
         <v>155</v>
@@ -4388,7 +4397,7 @@
       <c r="X45" s="14"/>
       <c r="Y45" s="6"/>
     </row>
-    <row r="46" spans="1:31">
+    <row r="46" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A46" s="28"/>
       <c r="B46" s="29" t="s">
         <v>156</v>
@@ -4441,7 +4450,7 @@
       <c r="W46" s="14"/>
       <c r="Z46" s="6"/>
     </row>
-    <row r="47" spans="1:31" s="6" customFormat="1">
+    <row r="47" spans="1:31" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A47" s="28"/>
       <c r="B47" s="29" t="s">
         <v>157</v>
@@ -4503,7 +4512,7 @@
       <c r="AD47"/>
       <c r="AE47"/>
     </row>
-    <row r="48" spans="1:31">
+    <row r="48" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A48" s="28"/>
       <c r="B48" s="29" t="s">
         <v>158</v>
@@ -4555,7 +4564,7 @@
       </c>
       <c r="W48" s="14"/>
     </row>
-    <row r="49" spans="1:31">
+    <row r="49" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A49" s="28"/>
       <c r="B49" s="29" t="s">
         <v>159</v>
@@ -4607,7 +4616,7 @@
       </c>
       <c r="W49" s="14"/>
     </row>
-    <row r="50" spans="1:31" s="6" customFormat="1">
+    <row r="50" spans="1:31" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A50" s="10"/>
       <c r="B50" s="22" t="s">
         <v>160</v>
@@ -4673,7 +4682,7 @@
       <c r="AD50"/>
       <c r="AE50"/>
     </row>
-    <row r="51" spans="1:31">
+    <row r="51" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A51" s="11" t="s">
         <v>115</v>
       </c>
@@ -4731,7 +4740,7 @@
       <c r="AD51" s="6"/>
       <c r="AE51" s="6"/>
     </row>
-    <row r="52" spans="1:31" s="6" customFormat="1">
+    <row r="52" spans="1:31" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A52" s="10"/>
       <c r="B52" s="22" t="s">
         <v>162</v>
@@ -4797,7 +4806,7 @@
       <c r="AD52"/>
       <c r="AE52"/>
     </row>
-    <row r="53" spans="1:31" s="6" customFormat="1">
+    <row r="53" spans="1:31" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A53" s="10"/>
       <c r="B53" s="22" t="s">
         <v>193</v>
@@ -4843,7 +4852,7 @@
       <c r="AD53" s="31"/>
       <c r="AE53" s="31"/>
     </row>
-    <row r="54" spans="1:31">
+    <row r="54" spans="1:31" x14ac:dyDescent="0.3">
       <c r="B54" s="22" t="s">
         <v>189</v>
       </c>
@@ -4873,7 +4882,7 @@
       <c r="W54" s="14"/>
       <c r="AB54" s="31"/>
     </row>
-    <row r="55" spans="1:31">
+    <row r="55" spans="1:31" x14ac:dyDescent="0.3">
       <c r="B55" s="22" t="s">
         <v>163</v>
       </c>
@@ -4928,7 +4937,7 @@
       <c r="W55" s="14"/>
       <c r="AB55" s="31"/>
     </row>
-    <row r="56" spans="1:31" s="31" customFormat="1">
+    <row r="56" spans="1:31" s="31" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A56" s="10"/>
       <c r="B56" s="22" t="s">
         <v>164</v>
@@ -4965,7 +4974,7 @@
       <c r="W56" s="14"/>
       <c r="X56" s="3"/>
     </row>
-    <row r="57" spans="1:31" s="31" customFormat="1">
+    <row r="57" spans="1:31" s="31" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A57" s="10"/>
       <c r="B57" s="22" t="s">
         <v>165</v>
@@ -5002,7 +5011,7 @@
       <c r="W57" s="14"/>
       <c r="X57" s="3"/>
     </row>
-    <row r="58" spans="1:31">
+    <row r="58" spans="1:31" x14ac:dyDescent="0.3">
       <c r="B58" s="22" t="s">
         <v>183</v>
       </c>
@@ -5039,7 +5048,7 @@
       <c r="Z58" s="6"/>
       <c r="AB58" s="31"/>
     </row>
-    <row r="59" spans="1:31">
+    <row r="59" spans="1:31" x14ac:dyDescent="0.3">
       <c r="B59" s="22" t="s">
         <v>166</v>
       </c>
@@ -5073,12 +5082,12 @@
       <c r="W59" s="14"/>
       <c r="AB59" s="31"/>
     </row>
-    <row r="60" spans="1:31">
+    <row r="60" spans="1:31" x14ac:dyDescent="0.3">
       <c r="B60" s="22" t="s">
         <v>167</v>
       </c>
       <c r="C60" s="13">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E60" s="13">
         <v>35</v>
@@ -5089,7 +5098,9 @@
       <c r="H60" s="13">
         <v>31</v>
       </c>
-      <c r="I60" s="21"/>
+      <c r="I60" s="21" t="s">
+        <v>211</v>
+      </c>
       <c r="J60" s="34">
         <v>1</v>
       </c>
@@ -5132,7 +5143,7 @@
       <c r="AA60" s="6"/>
       <c r="AB60" s="31"/>
     </row>
-    <row r="61" spans="1:31">
+    <row r="61" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A61" s="11" t="s">
         <v>114</v>
       </c>
@@ -5187,7 +5198,7 @@
       <c r="W61" s="14"/>
       <c r="AB61" s="31"/>
     </row>
-    <row r="62" spans="1:31">
+    <row r="62" spans="1:31" x14ac:dyDescent="0.3">
       <c r="B62" s="22" t="s">
         <v>169</v>
       </c>
@@ -5245,7 +5256,7 @@
       <c r="AD62" s="6"/>
       <c r="AE62" s="6"/>
     </row>
-    <row r="63" spans="1:31" s="31" customFormat="1">
+    <row r="63" spans="1:31" s="31" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A63" s="10"/>
       <c r="B63" s="22" t="s">
         <v>204</v>
@@ -5287,7 +5298,7 @@
       <c r="AD63" s="6"/>
       <c r="AE63" s="6"/>
     </row>
-    <row r="64" spans="1:31">
+    <row r="64" spans="1:31" x14ac:dyDescent="0.3">
       <c r="B64" s="22" t="s">
         <v>170</v>
       </c>
@@ -5342,7 +5353,7 @@
       <c r="W64" s="14"/>
       <c r="AB64" s="31"/>
     </row>
-    <row r="65" spans="1:31" s="31" customFormat="1">
+    <row r="65" spans="1:31" s="31" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A65" s="10"/>
       <c r="B65" s="22" t="s">
         <v>195</v>
@@ -5383,7 +5394,7 @@
       <c r="W65" s="14"/>
       <c r="X65" s="3"/>
     </row>
-    <row r="66" spans="1:31">
+    <row r="66" spans="1:31" x14ac:dyDescent="0.3">
       <c r="B66" s="22" t="s">
         <v>171</v>
       </c>
@@ -5403,7 +5414,7 @@
       <c r="AA66" s="6"/>
       <c r="AB66" s="31"/>
     </row>
-    <row r="67" spans="1:31">
+    <row r="67" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A67" s="11" t="s">
         <v>113</v>
       </c>
@@ -5448,7 +5459,7 @@
       <c r="W67" s="14"/>
       <c r="AB67" s="31"/>
     </row>
-    <row r="68" spans="1:31" s="31" customFormat="1">
+    <row r="68" spans="1:31" s="31" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A68" s="28"/>
       <c r="B68" s="29" t="s">
         <v>196</v>
@@ -5487,7 +5498,7 @@
       <c r="W68" s="14"/>
       <c r="X68" s="3"/>
     </row>
-    <row r="69" spans="1:31" s="31" customFormat="1">
+    <row r="69" spans="1:31" s="31" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A69" s="28"/>
       <c r="B69" s="29" t="s">
         <v>197</v>
@@ -5524,7 +5535,7 @@
       <c r="W69" s="14"/>
       <c r="X69" s="3"/>
     </row>
-    <row r="70" spans="1:31" s="31" customFormat="1">
+    <row r="70" spans="1:31" s="31" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A70" s="28"/>
       <c r="B70" s="29" t="s">
         <v>198</v>
@@ -5561,7 +5572,7 @@
       <c r="W70" s="14"/>
       <c r="X70" s="3"/>
     </row>
-    <row r="71" spans="1:31" s="31" customFormat="1">
+    <row r="71" spans="1:31" s="31" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A71" s="28"/>
       <c r="B71" s="29" t="s">
         <v>199</v>
@@ -5598,7 +5609,7 @@
       <c r="W71" s="14"/>
       <c r="X71" s="3"/>
     </row>
-    <row r="72" spans="1:31">
+    <row r="72" spans="1:31" x14ac:dyDescent="0.3">
       <c r="B72" s="22" t="s">
         <v>173</v>
       </c>
@@ -5628,7 +5639,7 @@
       </c>
       <c r="W72" s="14"/>
     </row>
-    <row r="73" spans="1:31">
+    <row r="73" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A73" s="11" t="s">
         <v>74</v>
       </c>
@@ -5676,7 +5687,7 @@
       </c>
       <c r="W73" s="14"/>
     </row>
-    <row r="74" spans="1:31" s="6" customFormat="1">
+    <row r="74" spans="1:31" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A74" s="28"/>
       <c r="B74" s="29" t="s">
         <v>82</v>
@@ -5730,7 +5741,7 @@
       <c r="AD74"/>
       <c r="AE74"/>
     </row>
-    <row r="75" spans="1:31">
+    <row r="75" spans="1:31" x14ac:dyDescent="0.3">
       <c r="B75" s="22" t="s">
         <v>93</v>
       </c>
@@ -5752,7 +5763,7 @@
       <c r="Y75" s="31"/>
       <c r="AA75" s="6"/>
     </row>
-    <row r="76" spans="1:31" s="31" customFormat="1">
+    <row r="76" spans="1:31" s="31" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A76" s="10"/>
       <c r="B76" s="22" t="s">
         <v>94</v>
@@ -5800,7 +5811,7 @@
       <c r="X76" s="3"/>
       <c r="AA76" s="6"/>
     </row>
-    <row r="77" spans="1:31">
+    <row r="77" spans="1:31" x14ac:dyDescent="0.3">
       <c r="B77" s="22" t="s">
         <v>177</v>
       </c>
@@ -5825,7 +5836,7 @@
       <c r="AD77" s="6"/>
       <c r="AE77" s="6"/>
     </row>
-    <row r="78" spans="1:31">
+    <row r="78" spans="1:31" x14ac:dyDescent="0.3">
       <c r="B78" s="22" t="s">
         <v>95</v>
       </c>
@@ -5863,7 +5874,7 @@
       </c>
       <c r="W78" s="14"/>
     </row>
-    <row r="79" spans="1:31" s="6" customFormat="1">
+    <row r="79" spans="1:31" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A79" s="10"/>
       <c r="B79" s="22" t="s">
         <v>96</v>
@@ -5917,7 +5928,7 @@
       <c r="AD79"/>
       <c r="AE79"/>
     </row>
-    <row r="80" spans="1:31" s="6" customFormat="1">
+    <row r="80" spans="1:31" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A80" s="10"/>
       <c r="B80" s="22" t="s">
         <v>206</v>
@@ -5963,7 +5974,7 @@
       <c r="AD80" s="31"/>
       <c r="AE80" s="31"/>
     </row>
-    <row r="81" spans="1:31">
+    <row r="81" spans="1:31" x14ac:dyDescent="0.3">
       <c r="B81" s="23" t="s">
         <v>97</v>
       </c>
@@ -6004,13 +6015,13 @@
       </c>
       <c r="W81" s="14"/>
     </row>
-    <row r="82" spans="1:31" ht="15" thickBot="1">
+    <row r="82" spans="1:31" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A82" s="11"/>
       <c r="V82" s="82"/>
       <c r="W82" s="14"/>
       <c r="Z82" s="31"/>
     </row>
-    <row r="83" spans="1:31">
+    <row r="83" spans="1:31" x14ac:dyDescent="0.3">
       <c r="I83" s="61" t="s">
         <v>98</v>
       </c>
@@ -6022,11 +6033,11 @@
       <c r="O83" s="62"/>
       <c r="P83" s="62">
         <f t="array" ref="P83">SUM($C2:$C81*(P2:P81&gt;=0.9)*($V2:$V81&gt;=$X$12))</f>
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="Q83" s="62">
         <f t="array" ref="Q83">SUM($C2:$C81*(Q2:Q81&gt;=0.9)*($V2:$V81&gt;=$X$12))</f>
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="R83" s="62"/>
       <c r="S83" s="62"/>
@@ -6038,7 +6049,7 @@
       <c r="AD83" s="6"/>
       <c r="AE83" s="6"/>
     </row>
-    <row r="84" spans="1:31">
+    <row r="84" spans="1:31" x14ac:dyDescent="0.3">
       <c r="I84" s="64" t="s">
         <v>100</v>
       </c>
@@ -6050,11 +6061,11 @@
       <c r="O84" s="65"/>
       <c r="P84" s="65">
         <f t="array" ref="P84">SUM($C2:$C81*P2:P81*($V2:$V81&gt;=$X$12))</f>
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="Q84" s="65">
         <f t="array" ref="Q84">SUM($C2:$C81*Q2:Q81*($V2:$V81&gt;=$X$12))</f>
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="R84" s="65"/>
       <c r="S84" s="65"/>
@@ -6062,7 +6073,7 @@
       <c r="U84" s="66"/>
       <c r="W84" s="14"/>
     </row>
-    <row r="85" spans="1:31" s="6" customFormat="1">
+    <row r="85" spans="1:31" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A85" s="10"/>
       <c r="B85" s="22"/>
       <c r="C85" s="13"/>
@@ -6082,11 +6093,11 @@
       <c r="O85" s="65"/>
       <c r="P85" s="65">
         <f t="array" ref="P85">SUM($C$2:$C$81*(P$2:P$81&gt;=0.1)*($V$2:$V$81&gt;=$X$12))</f>
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="Q85" s="65">
         <f t="array" ref="Q85">SUM($C$2:$C$81*(Q$2:Q$81&gt;=0.1)*($V$2:$V$81&gt;=$X$12))</f>
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="R85" s="65"/>
       <c r="S85" s="65"/>
@@ -6103,7 +6114,7 @@
       <c r="AD85"/>
       <c r="AE85"/>
     </row>
-    <row r="86" spans="1:31">
+    <row r="86" spans="1:31" x14ac:dyDescent="0.3">
       <c r="I86" s="64" t="s">
         <v>101</v>
       </c>
@@ -6115,11 +6126,11 @@
       <c r="O86" s="65"/>
       <c r="P86" s="65">
         <f t="shared" ref="P86:Q86" si="5">LOOKUP($X$12,$X23:$X31,$Y23:$Y31)</f>
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="Q86" s="65">
         <f t="shared" si="5"/>
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="R86" s="65"/>
       <c r="S86" s="65"/>
@@ -6131,7 +6142,7 @@
       <c r="AD86" s="6"/>
       <c r="AE86" s="6"/>
     </row>
-    <row r="87" spans="1:31">
+    <row r="87" spans="1:31" x14ac:dyDescent="0.3">
       <c r="I87" s="64" t="s">
         <v>102</v>
       </c>
@@ -6143,11 +6154,11 @@
       <c r="O87" s="67"/>
       <c r="P87" s="67">
         <f t="shared" ref="P87:Q87" si="6">P84/P86</f>
-        <v>0.81220657276995301</v>
+        <v>0.81132075471698117</v>
       </c>
       <c r="Q87" s="67">
         <f t="shared" si="6"/>
-        <v>0.53051643192488263</v>
+        <v>0.52830188679245282</v>
       </c>
       <c r="R87" s="67"/>
       <c r="S87" s="67"/>
@@ -6155,7 +6166,7 @@
       <c r="U87" s="68"/>
       <c r="W87" s="14"/>
     </row>
-    <row r="88" spans="1:31" ht="15" thickBot="1">
+    <row r="88" spans="1:31" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C88" s="31"/>
       <c r="I88" s="69" t="s">
         <v>80</v>
@@ -6184,59 +6195,59 @@
       <c r="AD88" s="6"/>
       <c r="AE88" s="6"/>
     </row>
-    <row r="89" spans="1:31">
+    <row r="89" spans="1:31" x14ac:dyDescent="0.3">
       <c r="C89" s="31"/>
       <c r="W89" s="14"/>
     </row>
-    <row r="90" spans="1:31">
+    <row r="90" spans="1:31" x14ac:dyDescent="0.3">
       <c r="C90" s="31"/>
       <c r="I90" s="13"/>
       <c r="J90" s="13"/>
       <c r="K90" s="13"/>
       <c r="W90" s="14"/>
     </row>
-    <row r="91" spans="1:31">
+    <row r="91" spans="1:31" x14ac:dyDescent="0.3">
       <c r="C91" s="31"/>
       <c r="I91" s="13"/>
       <c r="J91" s="13"/>
       <c r="K91" s="13"/>
       <c r="W91" s="14"/>
     </row>
-    <row r="92" spans="1:31">
+    <row r="92" spans="1:31" x14ac:dyDescent="0.3">
       <c r="I92" s="13"/>
       <c r="J92" s="13"/>
       <c r="K92" s="13"/>
       <c r="W92" s="14"/>
     </row>
-    <row r="93" spans="1:31">
+    <row r="93" spans="1:31" x14ac:dyDescent="0.3">
       <c r="I93" s="13"/>
       <c r="J93" s="13"/>
       <c r="K93" s="13"/>
       <c r="W93" s="14"/>
       <c r="AA93" s="31"/>
     </row>
-    <row r="94" spans="1:31">
+    <row r="94" spans="1:31" x14ac:dyDescent="0.3">
       <c r="I94" s="13"/>
       <c r="J94" s="13"/>
       <c r="K94" s="13"/>
       <c r="W94" s="14"/>
     </row>
-    <row r="95" spans="1:31">
+    <row r="95" spans="1:31" x14ac:dyDescent="0.3">
       <c r="I95" s="13"/>
       <c r="J95" s="13"/>
       <c r="K95" s="13"/>
     </row>
-    <row r="96" spans="1:31">
+    <row r="96" spans="1:31" x14ac:dyDescent="0.3">
       <c r="I96" s="13"/>
       <c r="J96" s="13"/>
       <c r="K96" s="13"/>
     </row>
-    <row r="97" spans="1:31">
+    <row r="97" spans="1:31" x14ac:dyDescent="0.3">
       <c r="I97" s="13"/>
       <c r="J97" s="13"/>
       <c r="K97" s="13"/>
     </row>
-    <row r="98" spans="1:31" s="31" customFormat="1">
+    <row r="98" spans="1:31" s="31" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A98" s="10"/>
       <c r="B98" s="22"/>
       <c r="C98" s="13"/>
@@ -6269,25 +6280,25 @@
       <c r="AD98"/>
       <c r="AE98"/>
     </row>
-    <row r="101" spans="1:31">
+    <row r="101" spans="1:31" x14ac:dyDescent="0.3">
       <c r="AB101" s="6"/>
       <c r="AC101" s="6"/>
       <c r="AD101" s="6"/>
       <c r="AE101" s="6"/>
     </row>
-    <row r="105" spans="1:31">
+    <row r="105" spans="1:31" x14ac:dyDescent="0.3">
       <c r="AB105" s="6"/>
       <c r="AC105" s="6"/>
       <c r="AD105" s="6"/>
       <c r="AE105" s="6"/>
     </row>
-    <row r="110" spans="1:31">
+    <row r="110" spans="1:31" x14ac:dyDescent="0.3">
       <c r="AB110" s="6"/>
       <c r="AC110" s="6"/>
       <c r="AD110" s="6"/>
       <c r="AE110" s="6"/>
     </row>
-    <row r="123" spans="28:31">
+    <row r="123" spans="28:31" x14ac:dyDescent="0.3">
       <c r="AB123" s="31"/>
       <c r="AC123" s="31"/>
       <c r="AD123" s="31"/>
@@ -6317,379 +6328,379 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:A73"/>
   <sheetViews>
     <sheetView topLeftCell="A43" workbookViewId="0">
       <selection sqref="A1:A73"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="50.1640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="50.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:1">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:1">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:1">
+    <row r="4" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:1">
+    <row r="5" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:1">
+    <row r="6" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:1">
+    <row r="7" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:1">
+    <row r="8" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="1:1">
+    <row r="9" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:1">
+    <row r="10" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="11" spans="1:1">
+    <row r="11" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="1:1">
+    <row r="12" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="13" spans="1:1">
+    <row r="13" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="14" spans="1:1">
+    <row r="14" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="15" spans="1:1">
+    <row r="15" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="16" spans="1:1">
+    <row r="16" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="17" spans="1:1">
+    <row r="17" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="18" spans="1:1">
+    <row r="18" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="19" spans="1:1">
+    <row r="19" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="20" spans="1:1">
+    <row r="20" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="21" spans="1:1">
+    <row r="21" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="22" spans="1:1">
+    <row r="22" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="23" spans="1:1">
+    <row r="23" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="24" spans="1:1">
+    <row r="24" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="25" spans="1:1">
+    <row r="25" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="26" spans="1:1">
+    <row r="26" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="27" spans="1:1">
+    <row r="27" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="28" spans="1:1">
+    <row r="28" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="29" spans="1:1">
+    <row r="29" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="30" spans="1:1">
+    <row r="30" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="31" spans="1:1">
+    <row r="31" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="32" spans="1:1">
+    <row r="32" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="33" spans="1:1">
+    <row r="33" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="34" spans="1:1">
+    <row r="34" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="35" spans="1:1">
+    <row r="35" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="36" spans="1:1">
+    <row r="36" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="37" spans="1:1">
+    <row r="37" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="38" spans="1:1">
+    <row r="38" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="39" spans="1:1">
+    <row r="39" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="40" spans="1:1">
+    <row r="40" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="41" spans="1:1">
+    <row r="41" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="42" spans="1:1">
+    <row r="42" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="43" spans="1:1">
+    <row r="43" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="44" spans="1:1">
+    <row r="44" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="45" spans="1:1">
+    <row r="45" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="46" spans="1:1">
+    <row r="46" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="47" spans="1:1">
+    <row r="47" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="48" spans="1:1">
+    <row r="48" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="49" spans="1:1">
+    <row r="49" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="50" spans="1:1">
+    <row r="50" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="51" spans="1:1">
+    <row r="51" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="52" spans="1:1">
+    <row r="52" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="53" spans="1:1">
+    <row r="53" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="54" spans="1:1">
+    <row r="54" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="55" spans="1:1">
+    <row r="55" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="56" spans="1:1">
+    <row r="56" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="57" spans="1:1">
+    <row r="57" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="58" spans="1:1">
+    <row r="58" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="59" spans="1:1">
+    <row r="59" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="60" spans="1:1">
+    <row r="60" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="61" spans="1:1">
+    <row r="61" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="62" spans="1:1">
+    <row r="62" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="63" spans="1:1">
+    <row r="63" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="64" spans="1:1">
+    <row r="64" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A64" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="65" spans="1:1">
+    <row r="65" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A65" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="66" spans="1:1">
+    <row r="66" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A66" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="67" spans="1:1">
+    <row r="67" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A67" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="68" spans="1:1">
+    <row r="68" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A68" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="69" spans="1:1">
+    <row r="69" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A69" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="70" spans="1:1">
+    <row r="70" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A70" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="71" spans="1:1">
+    <row r="71" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A71" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="72" spans="1:1">
+    <row r="72" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A72" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="73" spans="1:1">
+    <row r="73" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A73" t="s">
         <v>71</v>
       </c>

</xml_diff>